<commit_message>
Fixed some missing values
</commit_message>
<xml_diff>
--- a/source/solutions/stateElimination/ttc-evaluation-sheet-state-elimination-filled.xlsx
+++ b/source/solutions/stateElimination/ttc-evaluation-sheet-state-elimination-filled.xlsx
@@ -3092,7 +3092,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K13"/>
+      <selection activeCell="F14" sqref="F14:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3188,9 +3188,11 @@
         <v>31</v>
       </c>
       <c r="F3" s="57">
+        <v>4.17</v>
+      </c>
+      <c r="G3" s="54">
         <v>3</v>
       </c>
-      <c r="G3" s="54"/>
       <c r="H3" s="50" t="s">
         <v>32</v>
       </c>
@@ -3448,7 +3450,9 @@
         <v>30</v>
       </c>
       <c r="F14" s="57"/>
-      <c r="G14" s="54"/>
+      <c r="G14" s="54">
+        <v>3</v>
+      </c>
       <c r="H14" s="50" t="s">
         <v>30</v>
       </c>
@@ -3697,7 +3701,7 @@
       <c r="F26" s="27"/>
       <c r="G26" s="25">
         <f>SUM(G3:G25)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="27"/>
@@ -3720,7 +3724,7 @@
       </c>
       <c r="B28" s="29">
         <f>SUM(C26:M26)</f>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I28">
         <f>AVERAGE(I3:I13)</f>
@@ -3780,7 +3784,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J13"/>
+      <selection activeCell="G14" sqref="G14:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4138,7 +4142,9 @@
         <v>30</v>
       </c>
       <c r="F14" s="57"/>
-      <c r="G14" s="54"/>
+      <c r="G14" s="54">
+        <v>1</v>
+      </c>
       <c r="H14" s="50" t="s">
         <v>30</v>
       </c>
@@ -4387,7 +4393,7 @@
       <c r="F26" s="27"/>
       <c r="G26" s="25">
         <f>SUM(G3:G25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="27"/>
@@ -4410,7 +4416,7 @@
       </c>
       <c r="B28" s="29">
         <f>SUM(C26:M26)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I28">
         <f>AVERAGE(I3:I13)</f>

</xml_diff>